<commit_message>
Documentación - Corrección acorde al estándar
Se realiza la corrección de los entregables acorde al estándar de nomenclatura definido OSLO.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="100" windowWidth="18860" windowHeight="7300"/>
+    <workbookView xWindow="160" yWindow="100" windowWidth="18860" windowHeight="7300" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="91">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -855,6 +855,621 @@
   </si>
   <si>
     <t>Repetido</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ubicación: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositorio Testify\Fases_de_desarrollo\01-Inicio\01- Modelo de Negocios\IN04-OSLO- Modelo de Negocio.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nivel de gravedad: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ubicación: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositorio Testify\Fases_de_desarrollo\01-Inicio\01- Modelo de Negocios\IN04-OSLO-Modelo de Negocio.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\01-Inicio\01- Modelo de Negocios\IN05 -OSLO- Estudio de Factibilidad.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>Resumen de Entrevista 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\01-Inicio\01- Modelo de Negocios\IN07 -OSLO - Resumen de Entrevista 2.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\01-Inicio\02- Captura de Requerimientos\IN08 -OSLO - Propuesta de Desarrollo.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\E01 Plan de Iteración.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Pla de proyecto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\ELAB1-08-OSLO - Plan de Proyecto.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>Plan de Estimación</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nivel de gravedad: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio  Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\Plan de Estimación.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Plan de Calidad</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio  Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\E106-OSLO-Plan de Calidad.docx</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -945,7 +1560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -995,6 +1610,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1297,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1370,17 +1988,34 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:9" ht="58">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F3" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1"/>
@@ -1393,6 +2028,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1"/>
@@ -1405,6 +2041,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1"/>
@@ -1417,6 +2054,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
@@ -1429,6 +2067,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1"/>
@@ -1441,6 +2080,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9">
       <c r="B9" s="2">
@@ -1452,6 +2092,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9">
       <c r="B10" s="2">
@@ -1463,6 +2104,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" s="2">
@@ -1474,6 +2116,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9">
       <c r="B12" s="2">
@@ -1485,6 +2128,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="2">
@@ -1496,6 +2140,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" s="2">
@@ -1507,6 +2152,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="2">
@@ -1518,6 +2164,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" s="2">
@@ -1529,8 +2176,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" s="2">
         <v>16</v>
       </c>
@@ -1540,8 +2188,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" s="2">
         <v>17</v>
       </c>
@@ -1551,8 +2200,9 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" s="2">
         <v>18</v>
       </c>
@@ -1562,8 +2212,9 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20" s="2">
         <v>19</v>
       </c>
@@ -1573,8 +2224,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" s="2"/>
     </row>
     <row r="50" spans="1:1">
@@ -3906,8 +4558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4327,97 +4979,235 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:9" ht="58">
+      <c r="A15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F15" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="58">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="8"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="8"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="8"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="8"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="8"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="15"/>
+      <c r="E16" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F16" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="58">
+      <c r="A17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F17" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="58">
+      <c r="A18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F18" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="58">
+      <c r="A19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F19" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="58">
+      <c r="A20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F20" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="58">
+      <c r="A21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F21" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="58">
+      <c r="A22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F22" s="17">
+        <v>45551</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="8"/>

</xml_diff>

<commit_message>
Documentación - Correcion ortografica.
Se realiza revisión de ortografía en documento entregable cumpliendo con los estándares de calidad definidos en el plan SQA.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="96">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1609,6 +1609,73 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Repositorio  Testify\Main - Testify\Documentacion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\E105-OSLO-Herramientas y Tecnologias.docx</t>
     </r>
   </si>
 </sst>
@@ -4698,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I36" sqref="I33:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -5407,16 +5474,34 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="8"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="15"/>
+    <row r="25" spans="1:9" ht="58">
+      <c r="A25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.1516203703703702E-2</v>
+      </c>
+      <c r="F25" s="17">
+        <v>45553</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="8"/>

</xml_diff>

<commit_message>
Documentación - Informe Final SQA
Se añade el documento correspondiente al Informe Final SQA correspondiente a la Gestión de calidad.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="100" windowWidth="18860" windowHeight="7300" activeTab="7"/>
+    <workbookView xWindow="160" yWindow="100" windowWidth="18860" windowHeight="7300" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -2122,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4015,8 +4015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4765,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I36" sqref="I33:I36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4814,7 +4814,7 @@
         <v>64</v>
       </c>
       <c r="B2" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>75</v>
@@ -4843,7 +4843,7 @@
         <v>61</v>
       </c>
       <c r="B3" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>14</v>
@@ -4872,7 +4872,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>14</v>
@@ -4901,7 +4901,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>14</v>
@@ -4930,7 +4930,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
@@ -4959,7 +4959,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>14</v>
@@ -4988,7 +4988,7 @@
         <v>68</v>
       </c>
       <c r="B8" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Documentación - Se actualiza Plan de Calidad.
Se realizan correcciones ortográficas al documento del Plan de Calidad previa entrega.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="100">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1677,6 +1677,82 @@
       </rPr>
       <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\E105-OSLO-Herramientas y Tecnologias.docx</t>
     </r>
+  </si>
+  <si>
+    <t>Estándar OSLO, Ortográfico</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en el formato estándar definido por el grupo de desarrollo OSLO, errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de calidad\E107-OSLO-Plan de Calidad.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Tiempo empleado</t>
+  </si>
+  <si>
+    <t>Gestión de configuración</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1820,6 +1896,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4765,18 +4844,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
     <col min="9" max="9" width="99.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4787,14 +4868,14 @@
       <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>24</v>
@@ -4810,7 +4891,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="9">
@@ -4897,7 +4978,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="58">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="2">
@@ -5423,8 +5504,8 @@
       <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>14</v>
+      <c r="C23" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>15</v>
@@ -5503,16 +5584,32 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:9" ht="72.5">
+      <c r="A26" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="15"/>
+      <c r="C26" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="F26" s="17">
+        <v>45554</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="8"/>

</xml_diff>

<commit_message>
Documentación - Modificación plan de iteración Elaboración 2
Se realiza modificación del plan de iteración correspondiente a la fase de elaboración iteración 2.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="102">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1753,6 +1753,14 @@
   </si>
   <si>
     <t>Gestión de configuración</t>
+  </si>
+  <si>
+    <t>Plan Cierre iteracion fase Elaboracion iteracion 1</t>
+  </si>
+  <si>
+    <t>Descripción: Errores de ortografía.
+Nivel de gravedad: Leve.
+Ubicación: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\E103-OSLO-Plan de Iteración.docx</t>
   </si>
 </sst>
 </file>
@@ -4845,7 +4853,7 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="I34" sqref="I33:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5640,16 +5648,34 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="8"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="15"/>
+    <row r="28" spans="1:9" ht="60">
+      <c r="A28" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="2">
+        <v>26</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="F28" s="17">
+        <v>45559</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="8"/>

</xml_diff>

<commit_message>
Documentación - Actualización de Gestión SQA
Se realiza la actualización de los siguientes documentos: informe final de SQA para la fase de elaboración iteración 1 junto a su correspondiente documento en formato PDF, CheckListProductoClave, Nomenclaturas y se añade el informe final de SQA para la fase de elaboración iteración 2.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,21 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AE4DEC-2D5A-496E-977A-646BAAC13F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02C10F-BB5D-4DB2-B190-F44DC1BCF564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
-    <sheet name="MCU" sheetId="2" r:id="rId2"/>
-    <sheet name="MD" sheetId="3" r:id="rId3"/>
-    <sheet name="AdS" sheetId="4" r:id="rId4"/>
-    <sheet name="Pruebas" sheetId="5" r:id="rId5"/>
-    <sheet name="Riesgos" sheetId="6" r:id="rId6"/>
-    <sheet name="MdU" sheetId="7" r:id="rId7"/>
-    <sheet name="APOYO" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja1" sheetId="9" state="hidden" r:id="rId2"/>
+    <sheet name="MCU" sheetId="2" r:id="rId3"/>
+    <sheet name="MD" sheetId="3" r:id="rId4"/>
+    <sheet name="AdS" sheetId="4" r:id="rId5"/>
+    <sheet name="Pruebas" sheetId="5" r:id="rId6"/>
+    <sheet name="Riesgos" sheetId="6" r:id="rId7"/>
+    <sheet name="MdU" sheetId="7" r:id="rId8"/>
+    <sheet name="APOYO" sheetId="8" r:id="rId9"/>
+    <sheet name="RevisionesTotales" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -557,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="115">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -801,9 +816,6 @@
   </si>
   <si>
     <t>Tiempo empleado:</t>
-  </si>
-  <si>
-    <t>Estimación</t>
   </si>
   <si>
     <t>Descripción: Error encontrado en el formato estándar definido por el grupo de desarrollo OSLO para plantillas de uso cotidiano en el desarrollo de la aplicación Testify.
@@ -1780,6 +1792,39 @@
   </si>
   <si>
     <t>Índice no funcional</t>
+  </si>
+  <si>
+    <t>Documento</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>cantidad revisiones</t>
+  </si>
+  <si>
+    <t>cantidad documentos</t>
+  </si>
+  <si>
+    <t>Total revisiones</t>
+  </si>
+  <si>
+    <t>Cantidad de revisiones hechas</t>
+  </si>
+  <si>
+    <t>Documentos revisados en total</t>
+  </si>
+  <si>
+    <t>Confirmación</t>
+  </si>
+  <si>
+    <t>Documentos claves revisados en total</t>
+  </si>
+  <si>
+    <t>Fase Elaboracion Iteracion 1</t>
+  </si>
+  <si>
+    <t>Fase Elaboracion Iteracion 2</t>
   </si>
 </sst>
 </file>
@@ -1829,7 +1874,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1839,6 +1884,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1870,7 +1927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1926,6 +1983,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2236,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2319,7 @@
     <col min="9" max="9" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2281,8 +2347,11 @@
       <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2310,8 +2379,12 @@
       <c r="I2" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>COUNTIF(A2:A30,"*")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -2337,10 +2410,10 @@
         <v>19</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
@@ -2366,10 +2439,10 @@
         <v>19</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>4</v>
@@ -2382,7 +2455,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>5</v>
@@ -2395,7 +2468,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>6</v>
@@ -2408,7 +2481,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>7</v>
@@ -2421,7 +2494,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>8</v>
       </c>
@@ -2433,7 +2506,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>9</v>
       </c>
@@ -2445,7 +2518,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>10</v>
       </c>
@@ -2457,7 +2530,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -2469,7 +2542,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -2481,7 +2554,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -2493,7 +2566,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -2505,7 +2578,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -2595,12 +2668,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -2676,12 +2749,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I69"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7F18F4-1A82-4DA7-BAA1-7D801E9E7A78}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SUM(APOYO!N2,Riesgos!J2,MCU!J2,ERS!J2)</f>
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <f>SUM(APOYO!L2,Riesgos!J2,MCU!J2,ERS!J2)</f>
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>SUM(Riesgos!J2,ERS!J2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CA7489-87FD-4561-8F0C-4E8A76A52F34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J69"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,7 +2858,7 @@
     <col min="9" max="9" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2723,10 +2886,13 @@
       <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2750,10 +2916,14 @@
         <v>19</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="J2">
+        <f>COUNTIF(A2:A30,"*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -2764,7 +2934,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2">
         <v>3</v>
@@ -2776,7 +2946,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>4</v>
@@ -2788,7 +2958,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>5</v>
@@ -2800,7 +2970,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>6</v>
@@ -2812,7 +2982,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>7</v>
@@ -2824,7 +2994,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>8</v>
       </c>
@@ -2835,7 +3005,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>9</v>
       </c>
@@ -2846,7 +3016,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>10</v>
       </c>
@@ -2857,7 +3027,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -2868,7 +3038,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -2879,7 +3049,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -2890,7 +3060,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -2901,7 +3071,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -2983,12 +3153,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -3064,7 +3234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
@@ -3357,7 +3527,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -3432,7 +3602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
@@ -3725,7 +3895,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -3800,7 +3970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
@@ -4093,7 +4263,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4168,12 +4338,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4357,7 @@
     <col min="9" max="9" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4215,8 +4385,11 @@
       <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -4242,10 +4415,14 @@
         <v>19</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J2">
+        <f>COUNTIF(A2:A30,"*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -4256,7 +4433,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2">
         <v>3</v>
@@ -4268,7 +4445,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>4</v>
@@ -4280,7 +4457,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>5</v>
@@ -4292,7 +4469,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>6</v>
@@ -4304,7 +4481,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>7</v>
@@ -4316,7 +4493,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>8</v>
       </c>
@@ -4327,7 +4504,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>9</v>
       </c>
@@ -4338,7 +4515,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>10</v>
       </c>
@@ -4349,7 +4526,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -4360,7 +4537,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -4371,7 +4548,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -4382,7 +4559,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -4393,7 +4570,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -4475,7 +4652,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4550,12 +4727,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4843,7 +5020,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4918,12 +5095,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:I29"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4931,15 +5108,20 @@
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
     <col min="9" max="9" width="99.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4953,7 +5135,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>23</v>
@@ -4967,16 +5149,31 @@
       <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>14</v>
@@ -4994,12 +5191,31 @@
         <v>19</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Estudio e Implementación UARGFLOW*")</f>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f>SUM(K2:K17)</f>
+        <v>27</v>
+      </c>
+      <c r="M2">
+        <f>COUNTIF(A2:A67,"*")</f>
+        <v>27</v>
+      </c>
+      <c r="N2" s="20">
+        <f>COUNTIF($J$2:$J$28, "*")</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -5023,12 +5239,19 @@
         <v>19</v>
       </c>
       <c r="I3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de estimación*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -5052,12 +5275,19 @@
         <v>19</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Estudio de Factibilidad*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -5081,12 +5311,19 @@
         <v>19</v>
       </c>
       <c r="I5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="K5" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Informe Final de SQA*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -5110,12 +5347,19 @@
         <v>19</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Modelo de Negocio*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -5139,12 +5383,19 @@
         <v>19</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de Gestión de Configuración*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -5168,12 +5419,19 @@
         <v>19</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de Iteración*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -5197,12 +5455,19 @@
         <v>19</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de Proyecto (Ejemplo Gantt)*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -5226,12 +5491,19 @@
         <v>19</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de Proyecto*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -5255,12 +5527,19 @@
         <v>19</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Propuesta de Desarrollo*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -5284,12 +5563,19 @@
         <v>19</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Resumen de Entrevista*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -5313,12 +5599,19 @@
         <v>19</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Resumen de Reunión*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -5342,12 +5635,19 @@
         <v>19</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan de Calidad*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -5371,12 +5671,19 @@
         <v>19</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="20">
+        <f>COUNTIF($A$2:$A$28, "*GitHub*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -5398,12 +5705,19 @@
         <v>19</v>
       </c>
       <c r="I16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="20">
+        <f>COUNTIF($A$2:$A$27, "*Herramientas y Tecnologias*")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -5427,12 +5741,19 @@
         <v>19</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="20">
+        <f>COUNTIF($A$2:$A$28, "*Plan Cierre iteracion fase Elaboracion iteracion 1*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -5456,12 +5777,14 @@
         <v>19</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -5485,12 +5808,14 @@
         <v>19</v>
       </c>
       <c r="I19" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -5514,12 +5839,14 @@
         <v>19</v>
       </c>
       <c r="I20" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -5543,12 +5870,14 @@
         <v>19</v>
       </c>
       <c r="I21" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -5572,18 +5901,20 @@
         <v>19</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>14</v>
@@ -5601,12 +5932,14 @@
         <v>19</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -5630,18 +5963,19 @@
         <v>19</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>14</v>
@@ -5659,16 +5993,17 @@
         <v>19</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>14</v>
@@ -5686,12 +6021,13 @@
         <v>21</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2">
         <v>25</v>
@@ -5715,18 +6051,19 @@
         <v>19</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="2">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>14</v>
@@ -5744,10 +6081,11 @@
         <v>19</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="C31" s="8"/>
@@ -5756,8 +6094,9 @@
       <c r="F31" s="17"/>
       <c r="G31" s="3"/>
       <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="C32" s="8"/>
@@ -5767,8 +6106,9 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="C33" s="8"/>
@@ -5778,8 +6118,9 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="C34" s="8"/>
@@ -5789,8 +6130,9 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="15"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="C35" s="8"/>
@@ -5800,8 +6142,9 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="C36" s="8"/>
@@ -5811,8 +6154,9 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="15"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="C37" s="8"/>
@@ -5822,8 +6166,9 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="15"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="C38" s="8"/>
@@ -5833,8 +6178,9 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="15"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="8"/>
@@ -5844,8 +6190,9 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="C40" s="8"/>
@@ -5855,8 +6202,9 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="15"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="8"/>
@@ -5866,8 +6214,9 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="C42" s="8"/>
@@ -5877,8 +6226,9 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="C43" s="8"/>
@@ -5888,8 +6238,9 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="C44" s="8"/>
@@ -5899,8 +6250,9 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="15"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="15"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="C45" s="8"/>
@@ -5910,8 +6262,9 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="C46" s="8"/>
@@ -5921,8 +6274,9 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="15"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="C47" s="8"/>
@@ -5932,8 +6286,9 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="15"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="C48" s="8"/>
@@ -5943,8 +6298,9 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="15"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="15"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="C49" s="8"/>
@@ -5954,8 +6310,9 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="15"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="15"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="C50" s="8"/>
@@ -5965,8 +6322,9 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="C51" s="8"/>
@@ -5976,8 +6334,9 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="C52" s="8"/>
@@ -5987,8 +6346,9 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="C53" s="8"/>
@@ -5998,8 +6358,9 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="15"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="15"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="C54" s="8"/>
@@ -6009,8 +6370,9 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="15"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="C55" s="8"/>
@@ -6020,8 +6382,9 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="C56" s="8"/>
@@ -6031,8 +6394,9 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="C57" s="8"/>
@@ -6042,8 +6406,9 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="14"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="C58" s="8"/>
@@ -6053,8 +6418,9 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
@@ -6064,8 +6430,9 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="14"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
@@ -6075,8 +6442,9 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="C61" s="3"/>
@@ -6086,8 +6454,9 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="14"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
@@ -6097,8 +6466,9 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="14"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3"/>
@@ -6108,6 +6478,7 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">

</xml_diff>

<commit_message>
Documentación - Actualización Gestión SQA
Se realizan correcciones relacionadas al estándar OSLO definido por el equipo de desarrollo para nomenclatura de nombres sobre documentación/entregables correspondiente a las revisiones rutinarias.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02C10F-BB5D-4DB2-B190-F44DC1BCF564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B381F2A7-1043-4D29-B035-54960E7427CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="120">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -1825,6 +1825,88 @@
   </si>
   <si>
     <t>Fase Elaboracion Iteracion 2</t>
+  </si>
+  <si>
+    <t>Descripción: Se encontraron multiples conflictos de ramas para la sincronizacion local en el repositorio de Github.
+Nivel de gravedad: Moderado.
+Ubicación: Repositorio  Testify\Main - Testify\Documentacion</t>
+  </si>
+  <si>
+    <t>Prototipo</t>
+  </si>
+  <si>
+    <t>Revisión Rutinaria</t>
+  </si>
+  <si>
+    <t>Descripción: No se encontraron errores o incidentes.
+Ubicación: Repositorio  Testify\Main - \Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Prototipo Funcional Testify v1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Error encontrado en la nomenclatura para nombres definidos por el grupo de desarrollo OSLO (en total 6 archivos de reunión).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Repositorio \Testify\Registro_Reuniones</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1927,7 +2009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1990,6 +2072,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2304,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="C2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,14 +2848,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2809,14 +2893,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2843,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,8 +4058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4343,7 +4427,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5099,17 +5183,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
@@ -5206,7 +5290,7 @@
       </c>
       <c r="M2">
         <f>COUNTIF(A2:A67,"*")</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N2" s="20">
         <f>COUNTIF($J$2:$J$28, "*")</f>
@@ -6085,21 +6169,98 @@
       </c>
       <c r="J28" s="15"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="3"/>
-      <c r="I31" s="15"/>
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="2">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="23">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F29" s="22">
+        <v>45562</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="2">
+        <v>28</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F30" s="22">
+        <v>45564</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="F31" s="17">
+        <v>45564</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="8"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="3"/>
       <c r="E32" s="12"/>
       <c r="F32" s="17"/>
@@ -6111,7 +6272,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="8"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="3"/>
       <c r="E33" s="12"/>
       <c r="F33" s="17"/>
@@ -6123,7 +6284,7 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="8"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="3"/>
       <c r="E34" s="12"/>
       <c r="F34" s="17"/>
@@ -6135,7 +6296,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="8"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="3"/>
       <c r="E35" s="12"/>
       <c r="F35" s="17"/>
@@ -6147,7 +6308,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="8"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="3"/>
       <c r="E36" s="12"/>
       <c r="F36" s="17"/>
@@ -6159,7 +6320,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="8"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="3"/>
       <c r="E37" s="12"/>
       <c r="F37" s="17"/>
@@ -6171,7 +6332,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="8"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="3"/>
       <c r="E38" s="12"/>
       <c r="F38" s="17"/>
@@ -6183,7 +6344,7 @@
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="3"/>
       <c r="E39" s="12"/>
       <c r="F39" s="17"/>
@@ -6195,7 +6356,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="8"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="3"/>
       <c r="E40" s="12"/>
       <c r="F40" s="17"/>
@@ -6207,7 +6368,7 @@
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="8"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="3"/>
       <c r="E41" s="12"/>
       <c r="F41" s="17"/>
@@ -6480,6 +6641,141 @@
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
     </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+    </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>14</v>
@@ -6527,16 +6823,16 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Responsable" prompt="¿Que integrante del equipo de desarrollo realizo la revisión?" sqref="H32:H63 H2:H28" xr:uid="{00000000-0002-0000-0700-000004000000}">
+    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F31:F63 F2:F28" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C31:C63 C2:C28" xr:uid="{00000000-0002-0000-0700-000003000000}"/>
+    <dataValidation errorStyle="warning" showDropDown="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="E31:E63 E2:E28" xr:uid="{00000000-0002-0000-0700-000005000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Responsable" prompt="¿Que integrante del equipo de desarrollo realizo la revisión?" sqref="H2:H90" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>$A$107:$A$110</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="F31:F63 F2:F28" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="D31:D63 D2:D28" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="D2:D90" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>$A$100:$A$101</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C31:C63 C2:C28" xr:uid="{00000000-0002-0000-0700-000003000000}"/>
-    <dataValidation errorStyle="warning" showDropDown="1" showErrorMessage="1" errorTitle="No permitido" error="No se permite otra opción de chequeo." promptTitle="Chequeado" prompt="¿Fue este error chequeado?" sqref="E31:E63 E2:E28" xr:uid="{00000000-0002-0000-0700-000005000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otras opciones de resultado." promptTitle="Estado" prompt="¿Fue resuelto?" sqref="G31:G63 G2:G28" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otras opciones de resultado." promptTitle="Estado" prompt="¿Fue resuelto?" sqref="G2:G90" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>$A$103:$A$105</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Documentación - Revisión rutinaria SQA
Se realiza revisión rutinaria de documentos claves, se aplican correcciones ortográficas sobre el documento/entregable MCU.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B381F2A7-1043-4D29-B035-54960E7427CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224DA998-C14A-4DE9-AE0A-540CFF8104EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERS" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="121">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -818,22 +818,12 @@
     <t>Tiempo empleado:</t>
   </si>
   <si>
-    <t>Descripción: Error encontrado en el formato estándar definido por el grupo de desarrollo OSLO para plantillas de uso cotidiano en el desarrollo de la aplicación Testify.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio Testify/TEMPLATES</t>
-  </si>
-  <si>
     <t>Estudio de Factibilidad</t>
   </si>
   <si>
     <t>Estudio e Implementación UARGFLOW</t>
   </si>
   <si>
-    <t>Descripción: Error encontrado en el formato del nombre definido por el grupo de desarrollo OSLO para plantillas de uso cotidiano en el desarrollo de la aplicación Testify.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio Testify/TEMPLATES</t>
-  </si>
-  <si>
     <t>Informe Final de SQA</t>
   </si>
   <si>
@@ -862,11 +852,6 @@
   </si>
   <si>
     <t>Ortográfico</t>
-  </si>
-  <si>
-    <t>Descripción: Errores de ortografía.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio Testify/TEMPLATES</t>
   </si>
   <si>
     <t>Repetido</t>
@@ -1773,24 +1758,9 @@
     <t>Plan Cierre iteracion fase Elaboracion iteracion 1</t>
   </si>
   <si>
-    <t>Descripción: Errores de ortografía.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\E103-OSLO-Plan de Iteración.docx</t>
-  </si>
-  <si>
     <t>Modelo de caso de uso</t>
   </si>
   <si>
-    <t>Descripción: Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Modelo de casos de uso.docx</t>
-  </si>
-  <si>
-    <t>Descripción: Error encontrado en el funcionamiento del indice, se habia incluido una imagen completa como parte del indice en formato "titulo 2" haciendo que su funcionamiento no sea el correcto.
-Nivel de gravedad: Moderado.
-Ubicación: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\E104-OSLO-Especificación de Requerimientos.docx</t>
-  </si>
-  <si>
     <t>Índice no funcional</t>
   </si>
   <si>
@@ -1827,19 +1797,10 @@
     <t>Fase Elaboracion Iteracion 2</t>
   </si>
   <si>
-    <t>Descripción: Se encontraron multiples conflictos de ramas para la sincronizacion local en el repositorio de Github.
-Nivel de gravedad: Moderado.
-Ubicación: Repositorio  Testify\Main - Testify\Documentacion</t>
-  </si>
-  <si>
     <t>Prototipo</t>
   </si>
   <si>
     <t>Revisión Rutinaria</t>
-  </si>
-  <si>
-    <t>Descripción: No se encontraron errores o incidentes.
-Ubicación: Repositorio  Testify\Main - \Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Prototipo Funcional Testify v1</t>
   </si>
   <si>
     <r>
@@ -1906,6 +1867,587 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Repositorio \Testify\Registro_Reuniones</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en la nomenclatura definida por el grupo de desarrollo OSLO de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Modelo de casos de uso.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Errores de ortográfia.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Modelo de casos de uso.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en el funcionamiento del indice, se habia incluido una imagen completa como parte del indice en formato "titulo 2" haciendo que su funcionamiento no sea el correcto.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Moderado.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\E104-OSLO-Especificación de Requerimientos.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en el formato estándar definido por el grupo de desarrollo OSLO para plantillas de uso cotidiano en el desarrollo de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify/TEMPLATES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify\Fases_de_desarrollo\02-Elaboracion\05- Gestion de Proyecto\E103-OSLO-Plan de Iteración.docx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: No se encontraron errores o incidentes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio  Testify\Main - \Testify\Fases_de_desarrollo\02-Elaboracion\02- Analisis y Diseño\Prototipo Funcional Testify v1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Se encontraron multiples conflictos de ramas para la sincronizacion local en el repositorio de Github.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Moderado.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio  Testify\Main - Testify\Documentacion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error encontrado en el formato del nombre definido por el grupo de desarrollo OSLO para plantillas de uso cotidiano en el desarrollo de la aplicación Testify.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify/TEMPLATES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Errores de ortografía.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio Testify/TEMPLATES</t>
     </r>
   </si>
 </sst>
@@ -2389,7 +2931,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView topLeftCell="C2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2494,7 +3036,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2505,7 +3047,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
@@ -2523,7 +3065,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2752,12 +3294,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -2837,7 +3379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7F18F4-1A82-4DA7-BAA1-7D801E9E7A78}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2849,7 +3391,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -2859,18 +3401,18 @@
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2878,11 +3420,11 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>SUM(APOYO!N2,Riesgos!J2,MCU!J2,ERS!J2)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <f>SUM(APOYO!L2,Riesgos!J2,MCU!J2,ERS!J2)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2894,7 +3436,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -2927,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +3480,7 @@
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2971,12 +3513,12 @@
         <v>10</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3000,23 +3542,41 @@
         <v>19</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="J2">
         <f>COUNTIF(A2:A30,"*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="12">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="F3" s="17">
+        <v>45564</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -3237,12 +3797,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -3314,7 +3874,8 @@
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="No permitido" error="No se permiten otros tipos de verificaciones." promptTitle="Criterio de verificación" prompt="¿Que tipo de verificación involucra el error?" sqref="C2" xr:uid="{00000000-0002-0000-0700-000003000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3611,7 +4172,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -3979,7 +4540,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4347,7 +4908,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -4427,7 +4988,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4470,7 +5031,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4499,7 +5060,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="J2">
         <f>COUNTIF(A2:A30,"*")</f>
@@ -4736,7 +5297,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -5104,7 +5665,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -5183,8 +5744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5219,7 +5780,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>23</v>
@@ -5234,30 +5795,30 @@
         <v>10</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>14</v>
@@ -5275,10 +5836,10 @@
         <v>19</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" s="20">
         <f>COUNTIF($A$2:$A$28, "*Estudio e Implementación UARGFLOW*")</f>
@@ -5299,7 +5860,7 @@
     </row>
     <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -5323,10 +5884,10 @@
         <v>19</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K3" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de estimación*")</f>
@@ -5335,7 +5896,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -5359,10 +5920,10 @@
         <v>19</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="20">
         <f>COUNTIF($A$2:$A$28, "*Estudio de Factibilidad*")</f>
@@ -5371,7 +5932,7 @@
     </row>
     <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -5395,10 +5956,10 @@
         <v>19</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K5" s="20">
         <f>COUNTIF($A$2:$A$28, "*Informe Final de SQA*")</f>
@@ -5407,7 +5968,7 @@
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -5431,10 +5992,10 @@
         <v>19</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K6" s="20">
         <f>COUNTIF($A$2:$A$28, "*Modelo de Negocio*")</f>
@@ -5443,7 +6004,7 @@
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -5467,10 +6028,10 @@
         <v>19</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K7" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de Gestión de Configuración*")</f>
@@ -5479,7 +6040,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -5503,10 +6064,10 @@
         <v>19</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de Iteración*")</f>
@@ -5515,7 +6076,7 @@
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -5539,10 +6100,10 @@
         <v>19</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K9" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de Proyecto (Ejemplo Gantt)*")</f>
@@ -5551,7 +6112,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -5575,10 +6136,10 @@
         <v>19</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de Proyecto*")</f>
@@ -5587,7 +6148,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -5611,10 +6172,10 @@
         <v>19</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K11" s="20">
         <f>COUNTIF($A$2:$A$28, "*Propuesta de Desarrollo*")</f>
@@ -5623,7 +6184,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -5647,10 +6208,10 @@
         <v>19</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K12" s="20">
         <f>COUNTIF($A$2:$A$28, "*Resumen de Entrevista*")</f>
@@ -5659,7 +6220,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -5683,10 +6244,10 @@
         <v>19</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K13" s="20">
         <f>COUNTIF($A$2:$A$28, "*Resumen de Reunión*")</f>
@@ -5695,7 +6256,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -5719,10 +6280,10 @@
         <v>19</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K14" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan de Calidad*")</f>
@@ -5731,7 +6292,7 @@
     </row>
     <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -5755,10 +6316,10 @@
         <v>19</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K15" s="20">
         <f>COUNTIF($A$2:$A$28, "*GitHub*")</f>
@@ -5767,7 +6328,7 @@
     </row>
     <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -5789,10 +6350,10 @@
         <v>19</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K16" s="20">
         <f>COUNTIF($A$2:$A$27, "*Herramientas y Tecnologias*")</f>
@@ -5801,7 +6362,7 @@
     </row>
     <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -5825,10 +6386,10 @@
         <v>19</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K17" s="20">
         <f>COUNTIF($A$2:$A$28, "*Plan Cierre iteracion fase Elaboracion iteracion 1*")</f>
@@ -5837,7 +6398,7 @@
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -5861,14 +6422,14 @@
         <v>19</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -5892,14 +6453,14 @@
         <v>19</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -5923,14 +6484,14 @@
         <v>19</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -5954,14 +6515,14 @@
         <v>19</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -5985,20 +6546,20 @@
         <v>19</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>14</v>
@@ -6016,14 +6577,14 @@
         <v>19</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -6047,19 +6608,19 @@
         <v>19</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>14</v>
@@ -6077,17 +6638,17 @@
         <v>19</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>14</v>
@@ -6105,13 +6666,13 @@
         <v>21</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2">
         <v>25</v>
@@ -6135,19 +6696,19 @@
         <v>19</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B28" s="2">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>14</v>
@@ -6165,19 +6726,19 @@
         <v>19</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B29" s="2">
         <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>14</v>
@@ -6195,18 +6756,18 @@
         <v>19</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" s="2">
         <v>28</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>14</v>
@@ -6224,12 +6785,12 @@
         <v>19</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2">
         <v>29</v>
@@ -6253,7 +6814,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="J31" s="15"/>
     </row>

</xml_diff>

<commit_message>
Documentación - Actualización de reuniones y gestión SQA.
Se añaden los documentos 15 y 16 de reuniones correspondiente a la fase de elaboración iteración 2, se realiza revisión a los documentos 13, 14 y se modifican las fechas/hora mal establecidas.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1A9CB-68AB-4683-B999-49B3D5BABC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14885605-CF0E-46BA-8560-9511878A3DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="147">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -2518,6 +2518,17 @@
   </si>
   <si>
     <t>Cantidad de documentos</t>
+  </si>
+  <si>
+    <t>Resumen de Reunión 14</t>
+  </si>
+  <si>
+    <t>Resumen de Reunión 15</t>
+  </si>
+  <si>
+    <t>Descripción: Error en el establecimiento de las fechas/hora de reunión.
+Nivel de gravedad: Leve.
+Ubicación: Repositorio \Testify\Registro_Reuniones</t>
   </si>
 </sst>
 </file>
@@ -2964,15 +2975,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3028,6 +3030,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3885,38 +3896,38 @@
       <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="47" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51">
+      <c r="A3" s="48">
         <f>SUM(APOYO!O3,Riesgos!L2,ERS!L2)</f>
         <v>20</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="28">
         <f>SUM(APOYO!N3,Riesgos!L2,ERS!L2)</f>
-        <v>38</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31">
+        <v>40</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28">
         <v>2</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="29">
         <f>SUM(Riesgos!L2,ERS!L2)</f>
         <v>3</v>
       </c>
@@ -3934,11 +3945,11 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>SUM(APOYO!T3,MCU!M2,ERS!M2)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <f>SUM(APOYO!S3,MCU!L2,ERS!L3)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3989,7 +4000,7 @@
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4431,7 +4442,7 @@
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4814,7 +4825,7 @@
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5197,7 +5208,7 @@
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5580,7 +5591,7 @@
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -6004,7 +6015,7 @@
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -6371,7 +6382,7 @@
   <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I44" sqref="I42:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6425,20 +6436,20 @@
         <v>10</v>
       </c>
       <c r="J1" s="23"/>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="24" t="s">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="26"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="51"/>
     </row>
     <row r="2" spans="1:20" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -6469,34 +6480,34 @@
         <v>119</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="25" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6529,43 +6540,43 @@
         <v>114</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="31">
         <f>COUNTIF($A$2:$A$80, "*Estudio e Implementación UARGFLOW*")</f>
         <v>2</v>
       </c>
-      <c r="M3" s="35">
+      <c r="M3" s="32">
         <f>SUM(L3:L80)</f>
-        <v>35</v>
-      </c>
-      <c r="N3" s="35">
+        <v>37</v>
+      </c>
+      <c r="N3" s="32">
         <f>COUNTIF(A2:A80,"*")</f>
-        <v>35</v>
-      </c>
-      <c r="O3" s="36">
+        <v>37</v>
+      </c>
+      <c r="O3" s="33">
         <f>COUNTIF($K$3:$K$31, "*")</f>
         <v>17</v>
       </c>
-      <c r="P3" s="47" t="s">
+      <c r="P3" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" s="34">
+      <c r="Q3" s="31">
         <f>COUNTIF($A$2:$A$80, "*Prototipo*")</f>
         <v>1</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="32">
         <f>SUM(Q3:Q80)</f>
         <v>1</v>
       </c>
-      <c r="S3" s="35">
+      <c r="S3" s="32">
         <f>COUNTIF(A29:A90,"*")</f>
-        <v>8</v>
-      </c>
-      <c r="T3" s="35">
+        <v>10</v>
+      </c>
+      <c r="T3" s="32">
         <f>COUNTIF(A29:A90,"*")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -6597,21 +6608,21 @@
         <v>72</v>
       </c>
       <c r="J4" s="14"/>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="L4" s="38">
+      <c r="L4" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de estimación*")</f>
         <v>2</v>
       </c>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="37"/>
     </row>
     <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -6642,21 +6653,21 @@
         <v>118</v>
       </c>
       <c r="J5" s="13"/>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="35">
         <f>COUNTIF($A$2:$A$80, "*Estudio de Factibilidad*")</f>
         <v>2</v>
       </c>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="40"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="37"/>
     </row>
     <row r="6" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -6687,21 +6698,21 @@
         <v>114</v>
       </c>
       <c r="J6" s="13"/>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="38">
+      <c r="L6" s="35">
         <f>COUNTIF($A$2:$A$80, "*Informe Final de SQA*")</f>
         <v>1</v>
       </c>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="40"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="37"/>
     </row>
     <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -6732,21 +6743,21 @@
         <v>72</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="35">
         <f>COUNTIF($A$2:$A$80, "*Modelo de Negocio*")</f>
         <v>2</v>
       </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="40"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="37"/>
     </row>
     <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -6777,21 +6788,21 @@
         <v>72</v>
       </c>
       <c r="J8" s="15"/>
-      <c r="K8" s="42" t="s">
+      <c r="K8" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Gestión de Configuración*")</f>
         <v>1</v>
       </c>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="40"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="37"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -6822,21 +6833,21 @@
         <v>72</v>
       </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Iteración*")</f>
         <v>2</v>
       </c>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="40"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="37"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -6867,21 +6878,21 @@
         <v>72</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="42" t="s">
+      <c r="K10" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Proyecto (Ejemplo Gantt)*")</f>
         <v>1</v>
       </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="40"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="37"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -6912,21 +6923,21 @@
         <v>72</v>
       </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Proyecto*")</f>
         <v>2</v>
       </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="40"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="37"/>
     </row>
     <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -6957,21 +6968,21 @@
         <v>72</v>
       </c>
       <c r="J12" s="15"/>
-      <c r="K12" s="42" t="s">
+      <c r="K12" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L12" s="35">
         <f>COUNTIF($A$2:$A$80, "*Propuesta de Desarrollo*")</f>
         <v>2</v>
       </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="40"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="37"/>
     </row>
     <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -7002,21 +7013,21 @@
         <v>72</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="K13" s="42" t="s">
+      <c r="K13" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="38">
+      <c r="L13" s="35">
         <f>COUNTIF($A$2:$A$80, "*Resumen de Entrevista*")</f>
         <v>2</v>
       </c>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="40"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="37"/>
     </row>
     <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -7047,21 +7058,21 @@
         <v>72</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="42" t="s">
+      <c r="K14" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="L14" s="38">
+      <c r="L14" s="35">
         <f>COUNTIF($A$2:$A$80, "*Resumen de Reunión*")</f>
-        <v>8</v>
-      </c>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -7092,21 +7103,21 @@
         <v>74</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="42" t="s">
+      <c r="K15" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="38">
+      <c r="L15" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan de Calidad*")</f>
         <v>2</v>
       </c>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="40"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="37"/>
     </row>
     <row r="16" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -7135,21 +7146,21 @@
         <v>75</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="42" t="s">
+      <c r="K16" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="L16" s="38">
+      <c r="L16" s="35">
         <f>COUNTIF($A$2:$A$80, "*GitHub*")</f>
         <v>2</v>
       </c>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="40"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="37"/>
     </row>
     <row r="17" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -7180,21 +7191,21 @@
         <v>77</v>
       </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="42" t="s">
+      <c r="K17" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="38">
+      <c r="L17" s="35">
         <f>COUNTIF($A$2:$A$80, "*Herramientas y Tecnologias*")</f>
         <v>2</v>
       </c>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="40"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37"/>
     </row>
     <row r="18" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -7225,21 +7236,21 @@
         <v>78</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="42" t="s">
+      <c r="K18" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="35">
         <f>COUNTIF($A$2:$A$80, "*Plan Cierre iteracion fase Elaboracion iteracion 1*")</f>
         <v>1</v>
       </c>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="40"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="37"/>
     </row>
     <row r="19" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
@@ -7270,21 +7281,21 @@
         <v>79</v>
       </c>
       <c r="J19" s="15"/>
-      <c r="K19" s="43" t="s">
+      <c r="K19" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="L19" s="44">
+      <c r="L19" s="41">
         <f>COUNTIF($A$2:$A$80, "*Prototipo*")</f>
         <v>1</v>
       </c>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="46"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="43"/>
     </row>
     <row r="20" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -7813,29 +7824,65 @@
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="15"/>
+    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="2">
+        <v>35</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="12">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="F37" s="17">
+        <v>45569</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="15"/>
+    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="2">
+        <v>36</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="F38" s="17">
+        <v>45569</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
     </row>

</xml_diff>

<commit_message>
Documentación - Confección resumen de reunión 17 y gestión SQA
Se realiza resumen de reunión 17 y revisión rutinaria a los documentos de reunión.
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
+++ b/Fases_de_desarrollo/02-Elaboracion/07- Gestion de Calidad/ChecklistProductoClave.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\Fases_de_desarrollo\02-Elaboracion\07- Gestion de Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14885605-CF0E-46BA-8560-9511878A3DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A8C22A-05C9-4EC6-945B-3B4E104CE4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="150">
   <si>
     <t>Especificación de Requerimientos de Software.</t>
   </si>
@@ -2526,9 +2526,208 @@
     <t>Resumen de Reunión 15</t>
   </si>
   <si>
-    <t>Descripción: Error en el establecimiento de las fechas/hora de reunión.
-Nivel de gravedad: Leve.
-Ubicación: Repositorio \Testify\Registro_Reuniones</t>
+    <t>Resumen de Reunión 16</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error en el establecimiento de las fechas/hora de reunión.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio \Testify\Registro_Reuniones</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Error en el establecimiento de las fechas/hora de reunión.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio \Testify\Registro_Reuniones</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:Error encontrado en la nomenclatura para nombres definidos por el grupo de desarrollo OSLO 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel de gravedad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ubicación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Repositorio \Testify\Registro_Reuniones</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3920,7 +4119,7 @@
       </c>
       <c r="B3" s="28">
         <f>SUM(APOYO!N3,Riesgos!L2,ERS!L2)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -3945,11 +4144,11 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>SUM(APOYO!T3,MCU!M2,ERS!M2)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <f>SUM(APOYO!S3,MCU!L2,ERS!L3)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -6381,8 +6580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I44" sqref="I42:I44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6549,11 +6748,11 @@
       </c>
       <c r="M3" s="32">
         <f>SUM(L3:L80)</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N3" s="32">
         <f>COUNTIF(A2:A80,"*")</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O3" s="33">
         <f>COUNTIF($K$3:$K$31, "*")</f>
@@ -6572,11 +6771,11 @@
       </c>
       <c r="S3" s="32">
         <f>COUNTIF(A29:A90,"*")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T3" s="32">
         <f>COUNTIF(A29:A90,"*")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -7063,7 +7262,7 @@
       </c>
       <c r="L14" s="35">
         <f>COUNTIF($A$2:$A$80, "*Resumen de Reunión*")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
@@ -7850,7 +8049,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -7881,34 +8080,70 @@
         <v>19</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="15"/>
+    <row r="39" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="2">
+        <v>36</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F39" s="17">
+        <v>45574</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="15"/>
+    <row r="40" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="2">
+        <v>36</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="12">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F40" s="17">
+        <v>45574</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
     </row>

</xml_diff>